<commit_message>
Adapt queryString and hash on URL.
</commit_message>
<xml_diff>
--- a/meta/samples/pages/ValidationSample.xlsx
+++ b/meta/samples/pages/ValidationSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/samples/pages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512E10A5-D66C-2D4D-AD99-5E4303DF6C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8FB96C-E820-CE43-8FAC-36935A16DC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
   <si>
     <t>パッケージ</t>
   </si>
@@ -917,6 +917,18 @@
   </si>
   <si>
     <t>import { RouterHooks } from "@/utils/RouterHooks"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>qname</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>pname</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1563,27 +1575,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1592,38 +1603,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1635,8 +1639,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1669,18 +1673,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1690,12 +1692,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1709,19 +1711,19 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1734,22 +1736,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1767,13 +1769,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2189,8 +2191,8 @@
   </sheetPr>
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2234,9 +2236,6 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
@@ -2248,12 +2247,9 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="35"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
@@ -2265,12 +2261,9 @@
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="35"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
@@ -2282,12 +2275,9 @@
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
@@ -2297,99 +2287,81 @@
       <c r="C9" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="102" t="s">
+      <c r="A10" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="103"/>
+      <c r="B10" s="93"/>
       <c r="C10" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="102" t="s">
+      <c r="A11" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="103"/>
+      <c r="B11" s="93"/>
       <c r="C11" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="102" t="s">
+      <c r="A12" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="103"/>
+      <c r="B12" s="93"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="33"/>
+      <c r="D12" s="31"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="102" t="s">
+      <c r="A13" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="103"/>
-      <c r="C13" s="86" t="s">
+      <c r="B13" s="93"/>
+      <c r="C13" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="33"/>
+      <c r="D13" s="31"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="35"/>
     </row>
     <row r="14" spans="1:11" ht="45" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="105"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
@@ -2401,19 +2373,13 @@
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-    </row>
-    <row r="16" spans="1:11" s="32" customFormat="1">
-      <c r="A16" s="62" t="s">
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="64" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="55" t="s">
         <v>27</v>
       </c>
       <c r="D16" t="s">
@@ -2421,16 +2387,16 @@
       </c>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
+      <c r="G16"/>
+      <c r="H16"/>
       <c r="I16"/>
     </row>
-    <row r="17" spans="1:13" s="32" customFormat="1">
-      <c r="A17" s="62" t="s">
+    <row r="17" spans="1:12">
+      <c r="A17" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="64" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
@@ -2438,31 +2404,31 @@
       </c>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
+      <c r="G17"/>
+      <c r="H17"/>
       <c r="I17"/>
     </row>
-    <row r="18" spans="1:13" s="32" customFormat="1">
-      <c r="A18" s="62" t="s">
+    <row r="18" spans="1:12">
+      <c r="A18" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="55"/>
       <c r="D18" t="s">
         <v>36</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
+      <c r="G18"/>
+      <c r="H18"/>
       <c r="I18"/>
     </row>
-    <row r="19" spans="1:13" s="32" customFormat="1">
-      <c r="A19" s="62" t="s">
+    <row r="19" spans="1:12">
+      <c r="A19" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="64" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
@@ -2470,16 +2436,16 @@
       </c>
       <c r="E19"/>
       <c r="F19"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
+      <c r="G19"/>
+      <c r="H19"/>
       <c r="I19"/>
     </row>
-    <row r="20" spans="1:13" s="32" customFormat="1">
-      <c r="A20" s="62" t="s">
+    <row r="20" spans="1:12">
+      <c r="A20" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="64" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
@@ -2487,16 +2453,16 @@
       </c>
       <c r="E20"/>
       <c r="F20"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="66"/>
+      <c r="G20"/>
+      <c r="H20"/>
       <c r="I20"/>
     </row>
-    <row r="21" spans="1:13" s="32" customFormat="1">
-      <c r="A21" s="62" t="s">
+    <row r="21" spans="1:12">
+      <c r="A21" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
@@ -2504,16 +2470,16 @@
       </c>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
+      <c r="G21"/>
+      <c r="H21"/>
       <c r="I21"/>
     </row>
-    <row r="22" spans="1:13" s="32" customFormat="1">
-      <c r="A22" s="62" t="s">
+    <row r="22" spans="1:12">
+      <c r="A22" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="63"/>
-      <c r="C22" s="64" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
@@ -2521,31 +2487,31 @@
       </c>
       <c r="E22"/>
       <c r="F22"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
+      <c r="G22"/>
+      <c r="H22"/>
       <c r="I22"/>
     </row>
-    <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="94" t="s">
+    <row r="23" spans="1:12">
+      <c r="A23" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="95"/>
-      <c r="C23" s="64"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="55"/>
       <c r="D23" t="s">
         <v>58</v>
       </c>
       <c r="E23"/>
       <c r="F23"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
+      <c r="G23"/>
+      <c r="H23"/>
       <c r="I23"/>
     </row>
-    <row r="24" spans="1:13" s="32" customFormat="1">
-      <c r="A24" s="94" t="s">
+    <row r="24" spans="1:12">
+      <c r="A24" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="95"/>
-      <c r="C24" s="64" t="s">
+      <c r="B24" s="85"/>
+      <c r="C24" s="55" t="s">
         <v>97</v>
       </c>
       <c r="D24" t="s">
@@ -2557,27 +2523,27 @@
       <c r="H24"/>
       <c r="I24"/>
     </row>
-    <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="62" t="s">
+    <row r="25" spans="1:12">
+      <c r="A25" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="63"/>
-      <c r="C25" s="64" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
+      <c r="G25"/>
+      <c r="H25"/>
       <c r="I25"/>
     </row>
-    <row r="26" spans="1:13" s="32" customFormat="1">
-      <c r="A26" s="94" t="s">
+    <row r="26" spans="1:12">
+      <c r="A26" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="95"/>
-      <c r="C26" s="64" t="s">
+      <c r="B26" s="85"/>
+      <c r="C26" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D26" t="s">
@@ -2585,1279 +2551,1177 @@
       </c>
       <c r="E26"/>
       <c r="F26"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
+      <c r="G26"/>
+      <c r="H26"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:13" s="32" customFormat="1">
-      <c r="A27" s="94" t="s">
+    <row r="27" spans="1:12">
+      <c r="A27" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="95"/>
-      <c r="C27" s="64" t="s">
+      <c r="B27" s="85"/>
+      <c r="C27" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
+      <c r="G27"/>
+      <c r="H27"/>
       <c r="I27"/>
     </row>
-    <row r="28" spans="1:13" s="37" customFormat="1">
-      <c r="A28" s="34"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="30" t="s">
+    <row r="28" spans="1:12">
+      <c r="B28"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="44" t="s">
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="47" t="s">
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="35"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="51">
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="43">
         <v>1</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="35"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="51">
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="43">
         <v>2</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="35"/>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="51"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="35"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="51"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="35"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="52"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="35"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="30" t="s">
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="43"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="43"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="44"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="44" t="s">
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="43"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="47" t="s">
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="67"/>
-      <c r="I38" s="67"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="35"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="51">
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="43">
         <v>1</v>
       </c>
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="35"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="51">
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="43">
         <v>2</v>
       </c>
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="35"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="52">
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="44">
         <v>3</v>
       </c>
-      <c r="B41" s="48" t="s">
+      <c r="B41" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="49"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="35"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="83"/>
-      <c r="B42" s="67"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="35"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="83"/>
-      <c r="B43" s="67"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="35"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="30" t="s">
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="73"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="73"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="44" t="s">
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="43"/>
-      <c r="L44" s="43"/>
-      <c r="M44" s="43"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="47" t="s">
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="82"/>
-      <c r="F45" s="67"/>
-      <c r="G45" s="67"/>
-      <c r="H45" s="67"/>
-      <c r="I45" s="67"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="45"/>
-      <c r="M45" s="35"/>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="51"/>
-      <c r="B46" s="46"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="68"/>
-      <c r="G46" s="68"/>
-      <c r="H46" s="68"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="36"/>
-      <c r="K46" s="36"/>
-      <c r="L46" s="36"/>
-      <c r="M46" s="35"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="51"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="68"/>
-      <c r="G47" s="68"/>
-      <c r="H47" s="68"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="35"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="52"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="68"/>
-      <c r="H48" s="68"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="36"/>
-      <c r="K48" s="36"/>
-      <c r="L48" s="36"/>
-      <c r="M48" s="35"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="43"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="43"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="44"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="30" t="s">
+      <c r="A50" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="44" t="s">
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="71"/>
+      <c r="F50" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G50" s="44"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="44"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43"/>
-      <c r="M50" s="43"/>
     </row>
     <row r="51" spans="1:13">
-      <c r="A51" s="47" t="s">
+      <c r="A51" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="47" t="s">
+      <c r="C51" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="42" t="s">
+      <c r="D51" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="E51" s="82"/>
-      <c r="F51" s="67"/>
-      <c r="G51" s="67"/>
-      <c r="H51" s="67"/>
-      <c r="I51" s="67"/>
-      <c r="J51" s="44"/>
-      <c r="K51" s="45"/>
-      <c r="L51" s="45"/>
-      <c r="M51" s="35"/>
+      <c r="E51" s="72"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="51"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="87"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="68"/>
-      <c r="G52" s="68"/>
-      <c r="H52" s="68"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="36"/>
-      <c r="L52" s="36"/>
-      <c r="M52" s="35"/>
+      <c r="A52" s="43"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="77"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" s="51"/>
-      <c r="B53" s="46"/>
-      <c r="C53" s="88"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="68"/>
-      <c r="G53" s="68"/>
-      <c r="H53" s="68"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="36"/>
-      <c r="K53" s="36"/>
-      <c r="L53" s="36"/>
-      <c r="M53" s="35"/>
+      <c r="A53" s="43"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="78"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="52"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="89"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="36"/>
-      <c r="L54" s="36"/>
-      <c r="M54" s="35"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="79"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
     </row>
     <row r="55" spans="1:13">
-      <c r="A55" s="83"/>
-      <c r="B55" s="84"/>
-      <c r="C55" s="85"/>
-      <c r="D55" s="85"/>
-      <c r="E55" s="85"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="36"/>
-      <c r="L55" s="36"/>
-      <c r="M55" s="35"/>
+      <c r="A55" s="73"/>
+      <c r="B55" s="74"/>
+      <c r="C55" s="75"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="58"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="58"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="30" t="s">
+      <c r="A56" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="81"/>
-      <c r="F56" s="44" t="s">
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="71"/>
+      <c r="F56" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G56" s="44"/>
-      <c r="H56" s="44"/>
-      <c r="I56" s="44"/>
-      <c r="J56" s="43"/>
-      <c r="K56" s="43"/>
-      <c r="L56" s="43"/>
-      <c r="M56" s="43"/>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="47" t="s">
+      <c r="A57" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C57" s="42"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="82"/>
-      <c r="F57" s="67" t="s">
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="72"/>
+      <c r="F57" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="G57" s="67"/>
-      <c r="H57" s="67"/>
-      <c r="I57" s="67"/>
-      <c r="J57" s="44"/>
-      <c r="K57" s="45"/>
-      <c r="L57" s="45"/>
-      <c r="M57" s="35"/>
+      <c r="G57" s="57"/>
+      <c r="H57" s="57"/>
+      <c r="I57" s="57"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="37"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="51"/>
-      <c r="B58" s="46"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="68"/>
-      <c r="G58" s="68"/>
-      <c r="H58" s="68"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="36"/>
-      <c r="K58" s="36"/>
-      <c r="L58" s="36"/>
-      <c r="M58" s="35"/>
+      <c r="A58" s="43"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="58"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="51"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="68"/>
-      <c r="G59" s="68"/>
-      <c r="H59" s="68"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="36"/>
-      <c r="K59" s="36"/>
-      <c r="L59" s="36"/>
-      <c r="M59" s="35"/>
+      <c r="A59" s="43"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="58"/>
+      <c r="H59" s="58"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="52"/>
-      <c r="B60" s="48"/>
-      <c r="C60" s="49"/>
-      <c r="D60" s="49"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="68"/>
-      <c r="G60" s="68"/>
-      <c r="H60" s="68"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="36"/>
-      <c r="K60" s="36"/>
-      <c r="L60" s="36"/>
-      <c r="M60" s="35"/>
+      <c r="A60" s="44"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="58"/>
+      <c r="G60" s="58"/>
+      <c r="H60" s="58"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="13"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13" t="s">
+      <c r="A62"/>
+      <c r="B62" t="s">
         <v>61</v>
       </c>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62"/>
+      <c r="J62"/>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-      <c r="K63" s="14"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
       <c r="L63" s="6"/>
-      <c r="M63" s="15"/>
+      <c r="M63" s="14"/>
     </row>
     <row r="64" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A64" s="97" t="s">
+      <c r="A64" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="B64" s="97" t="s">
+      <c r="B64" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C64" s="96" t="s">
+      <c r="C64" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="96" t="s">
+      <c r="D64" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="96" t="s">
+      <c r="E64" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="100" t="s">
+      <c r="F64" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="G64" s="100" t="s">
+      <c r="G64" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="H64" s="98" t="s">
+      <c r="H64" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="I64" s="96" t="s">
+      <c r="I64" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="J64" s="96"/>
-      <c r="K64" s="16"/>
-      <c r="L64" s="17"/>
+      <c r="J64" s="86"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="16"/>
       <c r="M64" s="9"/>
     </row>
     <row r="65" spans="1:13">
-      <c r="A65" s="97"/>
-      <c r="B65" s="97"/>
-      <c r="C65" s="96"/>
-      <c r="D65" s="96"/>
-      <c r="E65" s="96"/>
-      <c r="F65" s="101"/>
-      <c r="G65" s="101"/>
-      <c r="H65" s="99"/>
-      <c r="I65" s="96"/>
-      <c r="J65" s="96"/>
-      <c r="K65" s="18"/>
-      <c r="L65" s="29"/>
-      <c r="M65" s="15"/>
+      <c r="A65" s="87"/>
+      <c r="B65" s="87"/>
+      <c r="C65" s="86"/>
+      <c r="D65" s="86"/>
+      <c r="E65" s="86"/>
+      <c r="F65" s="91"/>
+      <c r="G65" s="91"/>
+      <c r="H65" s="89"/>
+      <c r="I65" s="86"/>
+      <c r="J65" s="86"/>
+      <c r="K65" s="17"/>
+      <c r="L65" s="28"/>
+      <c r="M65" s="14"/>
     </row>
     <row r="66" spans="1:13">
-      <c r="A66" s="19">
+      <c r="A66" s="18">
         <v>1</v>
       </c>
-      <c r="B66" s="71"/>
-      <c r="C66" s="78"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="69"/>
-      <c r="H66" s="69"/>
-      <c r="I66" s="20"/>
-      <c r="J66" s="21"/>
-      <c r="K66" s="21"/>
-      <c r="L66" s="28"/>
-      <c r="M66" s="15"/>
+      <c r="B66" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="I66" s="19"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="27"/>
+      <c r="M66" s="14"/>
     </row>
     <row r="67" spans="1:13">
-      <c r="A67" s="19">
+      <c r="A67" s="18">
         <f>A66+1</f>
         <v>2</v>
       </c>
-      <c r="B67" s="71"/>
-      <c r="C67" s="78"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="69"/>
-      <c r="H67" s="69"/>
-      <c r="I67" s="20"/>
-      <c r="J67" s="21"/>
-      <c r="K67" s="21"/>
-      <c r="L67" s="28"/>
-      <c r="M67" s="15"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="59"/>
+      <c r="H67" s="59"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="20"/>
+      <c r="K67" s="20"/>
+      <c r="L67" s="27"/>
+      <c r="M67" s="14"/>
     </row>
     <row r="68" spans="1:13">
-      <c r="A68" s="19">
+      <c r="A68" s="18">
         <f t="shared" ref="A68:A82" si="0">A67+1</f>
         <v>3</v>
       </c>
-      <c r="B68" s="72"/>
-      <c r="C68" s="79"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="69"/>
-      <c r="H68" s="69"/>
-      <c r="I68" s="20"/>
-      <c r="J68" s="21"/>
-      <c r="K68" s="21"/>
-      <c r="L68" s="22"/>
-      <c r="M68" s="15"/>
+      <c r="B68" s="62"/>
+      <c r="C68" s="69"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="59"/>
+      <c r="H68" s="59"/>
+      <c r="I68" s="19"/>
+      <c r="J68" s="20"/>
+      <c r="K68" s="20"/>
+      <c r="L68" s="21"/>
+      <c r="M68" s="14"/>
     </row>
     <row r="69" spans="1:13">
-      <c r="A69" s="19">
+      <c r="A69" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B69" s="73"/>
-      <c r="C69" s="80"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="69"/>
-      <c r="H69" s="69"/>
-      <c r="I69" s="20"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="21"/>
-      <c r="L69" s="22"/>
-      <c r="M69" s="15"/>
+      <c r="B69" s="63"/>
+      <c r="C69" s="70"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="59"/>
+      <c r="H69" s="59"/>
+      <c r="I69" s="19"/>
+      <c r="J69" s="20"/>
+      <c r="K69" s="20"/>
+      <c r="L69" s="21"/>
+      <c r="M69" s="14"/>
     </row>
     <row r="70" spans="1:13">
-      <c r="A70" s="19">
+      <c r="A70" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B70" s="73"/>
-      <c r="C70" s="80"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="69"/>
-      <c r="H70" s="69"/>
-      <c r="I70" s="20"/>
-      <c r="J70" s="21"/>
-      <c r="K70" s="21"/>
-      <c r="L70" s="22"/>
-      <c r="M70" s="15"/>
+      <c r="B70" s="63"/>
+      <c r="C70" s="70"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="59"/>
+      <c r="H70" s="59"/>
+      <c r="I70" s="19"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="21"/>
+      <c r="M70" s="14"/>
     </row>
     <row r="71" spans="1:13">
-      <c r="A71" s="19">
+      <c r="A71" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B71" s="73"/>
-      <c r="C71" s="80"/>
-      <c r="D71" s="74"/>
-      <c r="E71" s="74"/>
-      <c r="F71" s="74"/>
-      <c r="G71" s="75"/>
-      <c r="H71" s="75"/>
-      <c r="I71" s="74"/>
-      <c r="J71" s="76"/>
-      <c r="K71" s="76"/>
-      <c r="L71" s="77"/>
-      <c r="M71" s="15"/>
+      <c r="B71" s="63"/>
+      <c r="C71" s="70"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="65"/>
+      <c r="H71" s="65"/>
+      <c r="I71" s="64"/>
+      <c r="J71" s="66"/>
+      <c r="K71" s="66"/>
+      <c r="L71" s="67"/>
+      <c r="M71" s="14"/>
     </row>
     <row r="72" spans="1:13">
-      <c r="A72" s="19">
+      <c r="A72" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B72" s="73"/>
-      <c r="C72" s="80"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="20"/>
-      <c r="G72" s="69"/>
-      <c r="H72" s="69"/>
-      <c r="I72" s="20"/>
-      <c r="J72" s="21"/>
-      <c r="K72" s="21"/>
-      <c r="L72" s="22"/>
-      <c r="M72" s="15"/>
+      <c r="B72" s="63"/>
+      <c r="C72" s="70"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="59"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="19"/>
+      <c r="J72" s="20"/>
+      <c r="K72" s="20"/>
+      <c r="L72" s="21"/>
+      <c r="M72" s="14"/>
     </row>
     <row r="73" spans="1:13">
-      <c r="A73" s="19">
+      <c r="A73" s="18">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B73" s="73"/>
-      <c r="C73" s="80"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-      <c r="F73" s="74"/>
-      <c r="G73" s="75"/>
-      <c r="H73" s="75"/>
-      <c r="I73" s="74"/>
-      <c r="J73" s="76"/>
-      <c r="K73" s="76"/>
-      <c r="L73" s="77"/>
-      <c r="M73" s="15"/>
+      <c r="B73" s="63"/>
+      <c r="C73" s="70"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="65"/>
+      <c r="H73" s="65"/>
+      <c r="I73" s="64"/>
+      <c r="J73" s="66"/>
+      <c r="K73" s="66"/>
+      <c r="L73" s="67"/>
+      <c r="M73" s="14"/>
     </row>
     <row r="74" spans="1:13">
-      <c r="A74" s="19">
+      <c r="A74" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B74" s="73"/>
-      <c r="C74" s="80"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="75"/>
-      <c r="H74" s="75"/>
-      <c r="I74" s="74"/>
-      <c r="J74" s="76"/>
-      <c r="K74" s="76"/>
-      <c r="L74" s="77"/>
-      <c r="M74" s="15"/>
+      <c r="B74" s="63"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="65"/>
+      <c r="H74" s="65"/>
+      <c r="I74" s="64"/>
+      <c r="J74" s="66"/>
+      <c r="K74" s="66"/>
+      <c r="L74" s="67"/>
+      <c r="M74" s="14"/>
     </row>
     <row r="75" spans="1:13">
-      <c r="A75" s="19">
+      <c r="A75" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B75" s="73"/>
-      <c r="C75" s="80"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
-      <c r="G75" s="69"/>
-      <c r="H75" s="69"/>
-      <c r="I75" s="20"/>
-      <c r="J75" s="21"/>
-      <c r="K75" s="21"/>
-      <c r="L75" s="22"/>
-      <c r="M75" s="15"/>
+      <c r="B75" s="63"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="59"/>
+      <c r="H75" s="59"/>
+      <c r="I75" s="19"/>
+      <c r="J75" s="20"/>
+      <c r="K75" s="20"/>
+      <c r="L75" s="21"/>
+      <c r="M75" s="14"/>
     </row>
     <row r="76" spans="1:13">
-      <c r="A76" s="19">
+      <c r="A76" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B76" s="73"/>
-      <c r="C76" s="80"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="75"/>
-      <c r="H76" s="75"/>
-      <c r="I76" s="74"/>
-      <c r="J76" s="76"/>
-      <c r="K76" s="76"/>
-      <c r="L76" s="77"/>
-      <c r="M76" s="15"/>
+      <c r="B76" s="63"/>
+      <c r="C76" s="70"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="65"/>
+      <c r="H76" s="65"/>
+      <c r="I76" s="64"/>
+      <c r="J76" s="66"/>
+      <c r="K76" s="66"/>
+      <c r="L76" s="67"/>
+      <c r="M76" s="14"/>
     </row>
     <row r="77" spans="1:13">
-      <c r="A77" s="19">
+      <c r="A77" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B77" s="73"/>
-      <c r="C77" s="80"/>
-      <c r="D77" s="74"/>
-      <c r="E77" s="74"/>
-      <c r="F77" s="74"/>
-      <c r="G77" s="75"/>
-      <c r="H77" s="75"/>
-      <c r="I77" s="74"/>
-      <c r="J77" s="76"/>
-      <c r="K77" s="76"/>
-      <c r="L77" s="77"/>
-      <c r="M77" s="15"/>
+      <c r="B77" s="63"/>
+      <c r="C77" s="70"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="64"/>
+      <c r="F77" s="64"/>
+      <c r="G77" s="65"/>
+      <c r="H77" s="65"/>
+      <c r="I77" s="64"/>
+      <c r="J77" s="66"/>
+      <c r="K77" s="66"/>
+      <c r="L77" s="67"/>
+      <c r="M77" s="14"/>
     </row>
     <row r="78" spans="1:13">
-      <c r="A78" s="19">
+      <c r="A78" s="18">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B78" s="73"/>
-      <c r="C78" s="80"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="69"/>
-      <c r="H78" s="69"/>
-      <c r="I78" s="20"/>
-      <c r="J78" s="21"/>
-      <c r="K78" s="21"/>
-      <c r="L78" s="22"/>
-      <c r="M78" s="15"/>
+      <c r="B78" s="63"/>
+      <c r="C78" s="70"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="59"/>
+      <c r="H78" s="59"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="20"/>
+      <c r="K78" s="20"/>
+      <c r="L78" s="21"/>
+      <c r="M78" s="14"/>
     </row>
     <row r="79" spans="1:13">
-      <c r="A79" s="19">
+      <c r="A79" s="18">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B79" s="73"/>
-      <c r="C79" s="80"/>
-      <c r="D79" s="74"/>
-      <c r="E79" s="74"/>
-      <c r="F79" s="74"/>
-      <c r="G79" s="75"/>
-      <c r="H79" s="75"/>
-      <c r="I79" s="74"/>
-      <c r="J79" s="76"/>
-      <c r="K79" s="76"/>
-      <c r="L79" s="77"/>
-      <c r="M79" s="15"/>
+      <c r="B79" s="63"/>
+      <c r="C79" s="70"/>
+      <c r="D79" s="64"/>
+      <c r="E79" s="64"/>
+      <c r="F79" s="64"/>
+      <c r="G79" s="65"/>
+      <c r="H79" s="65"/>
+      <c r="I79" s="64"/>
+      <c r="J79" s="66"/>
+      <c r="K79" s="66"/>
+      <c r="L79" s="67"/>
+      <c r="M79" s="14"/>
     </row>
     <row r="80" spans="1:13">
-      <c r="A80" s="19">
+      <c r="A80" s="18">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B80" s="73"/>
-      <c r="C80" s="80"/>
-      <c r="D80" s="74"/>
-      <c r="E80" s="74"/>
-      <c r="F80" s="74"/>
-      <c r="G80" s="75"/>
-      <c r="H80" s="75"/>
-      <c r="I80" s="74"/>
-      <c r="J80" s="76"/>
-      <c r="K80" s="76"/>
-      <c r="L80" s="77"/>
-      <c r="M80" s="15"/>
+      <c r="B80" s="63"/>
+      <c r="C80" s="70"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="64"/>
+      <c r="G80" s="65"/>
+      <c r="H80" s="65"/>
+      <c r="I80" s="64"/>
+      <c r="J80" s="66"/>
+      <c r="K80" s="66"/>
+      <c r="L80" s="67"/>
+      <c r="M80" s="14"/>
     </row>
     <row r="81" spans="1:13">
-      <c r="A81" s="19">
+      <c r="A81" s="18">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B81" s="73"/>
-      <c r="C81" s="80"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="20"/>
-      <c r="G81" s="69"/>
-      <c r="H81" s="69"/>
-      <c r="I81" s="20"/>
-      <c r="J81" s="21"/>
-      <c r="K81" s="21"/>
-      <c r="L81" s="22"/>
-      <c r="M81" s="15"/>
+      <c r="B81" s="63"/>
+      <c r="C81" s="70"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="59"/>
+      <c r="H81" s="59"/>
+      <c r="I81" s="19"/>
+      <c r="J81" s="20"/>
+      <c r="K81" s="20"/>
+      <c r="L81" s="21"/>
+      <c r="M81" s="14"/>
     </row>
     <row r="82" spans="1:13">
-      <c r="A82" s="19">
+      <c r="A82" s="18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B82" s="73"/>
-      <c r="C82" s="80"/>
-      <c r="D82" s="74"/>
-      <c r="E82" s="74"/>
-      <c r="F82" s="74"/>
-      <c r="G82" s="75"/>
-      <c r="H82" s="75"/>
-      <c r="I82" s="74"/>
-      <c r="J82" s="76"/>
-      <c r="K82" s="76"/>
-      <c r="L82" s="77"/>
-      <c r="M82" s="15"/>
+      <c r="B82" s="63"/>
+      <c r="C82" s="70"/>
+      <c r="D82" s="64"/>
+      <c r="E82" s="64"/>
+      <c r="F82" s="64"/>
+      <c r="G82" s="65"/>
+      <c r="H82" s="65"/>
+      <c r="I82" s="64"/>
+      <c r="J82" s="66"/>
+      <c r="K82" s="66"/>
+      <c r="L82" s="67"/>
+      <c r="M82" s="14"/>
     </row>
     <row r="83" spans="1:13">
-      <c r="A83" s="23"/>
-      <c r="B83" s="24"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="25"/>
-      <c r="G83" s="70"/>
-      <c r="H83" s="70"/>
-      <c r="I83" s="25"/>
-      <c r="J83" s="26"/>
-      <c r="K83" s="26"/>
-      <c r="L83" s="27"/>
-      <c r="M83" s="15"/>
+      <c r="A83" s="22"/>
+      <c r="B83" s="23"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="60"/>
+      <c r="H83" s="60"/>
+      <c r="I83" s="24"/>
+      <c r="J83" s="25"/>
+      <c r="K83" s="25"/>
+      <c r="L83" s="26"/>
+      <c r="M83" s="14"/>
     </row>
     <row r="85" spans="1:13">
-      <c r="A85" s="30" t="s">
+      <c r="A85" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B85" s="31"/>
-      <c r="C85" s="31"/>
-      <c r="D85" s="31"/>
-      <c r="E85" s="81"/>
-      <c r="F85" s="44" t="s">
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="71"/>
+      <c r="F85" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G85" s="44"/>
-      <c r="H85" s="44"/>
-      <c r="I85" s="44"/>
-      <c r="J85" s="43"/>
-      <c r="K85" s="43"/>
-      <c r="L85" s="43"/>
-      <c r="M85" s="43"/>
     </row>
     <row r="86" spans="1:13">
-      <c r="A86" s="47" t="s">
+      <c r="A86" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B86" s="42" t="s">
+      <c r="B86" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C86" s="42"/>
-      <c r="D86" s="42"/>
-      <c r="E86" s="82"/>
-      <c r="F86" s="67"/>
-      <c r="G86" s="67"/>
-      <c r="H86" s="67"/>
-      <c r="I86" s="67"/>
-      <c r="J86" s="44"/>
-      <c r="K86" s="45"/>
-      <c r="L86" s="45"/>
-      <c r="M86" s="35"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="36"/>
+      <c r="E86" s="72"/>
+      <c r="F86" s="57"/>
+      <c r="G86" s="57"/>
+      <c r="H86" s="57"/>
+      <c r="I86" s="57"/>
+      <c r="K86" s="37"/>
+      <c r="L86" s="37"/>
     </row>
     <row r="87" spans="1:13">
-      <c r="A87" s="51"/>
-      <c r="B87" s="46"/>
-      <c r="C87" s="38"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="39"/>
-      <c r="F87" s="68"/>
-      <c r="G87" s="68"/>
-      <c r="H87" s="68"/>
-      <c r="I87" s="34"/>
-      <c r="J87" s="36"/>
-      <c r="K87" s="36"/>
-      <c r="L87" s="36"/>
-      <c r="M87" s="35"/>
+      <c r="A87" s="43"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="33"/>
+      <c r="F87" s="58"/>
+      <c r="G87" s="58"/>
+      <c r="H87" s="58"/>
+      <c r="J87"/>
+      <c r="K87"/>
+      <c r="L87"/>
     </row>
     <row r="88" spans="1:13">
-      <c r="A88" s="51"/>
-      <c r="B88" s="46"/>
-      <c r="C88" s="40"/>
-      <c r="D88" s="40"/>
-      <c r="E88" s="41"/>
-      <c r="F88" s="68"/>
-      <c r="G88" s="68"/>
-      <c r="H88" s="68"/>
-      <c r="I88" s="34"/>
-      <c r="J88" s="36"/>
-      <c r="K88" s="36"/>
-      <c r="L88" s="36"/>
-      <c r="M88" s="35"/>
+      <c r="A88" s="43"/>
+      <c r="B88" s="38"/>
+      <c r="C88" s="34"/>
+      <c r="D88" s="34"/>
+      <c r="E88" s="35"/>
+      <c r="F88" s="58"/>
+      <c r="G88" s="58"/>
+      <c r="H88" s="58"/>
+      <c r="J88"/>
+      <c r="K88"/>
+      <c r="L88"/>
     </row>
     <row r="89" spans="1:13">
-      <c r="A89" s="52"/>
-      <c r="B89" s="48"/>
-      <c r="C89" s="49"/>
-      <c r="D89" s="49"/>
-      <c r="E89" s="50"/>
-      <c r="F89" s="68"/>
-      <c r="G89" s="68"/>
-      <c r="H89" s="68"/>
-      <c r="I89" s="34"/>
-      <c r="J89" s="36"/>
-      <c r="K89" s="36"/>
-      <c r="L89" s="36"/>
-      <c r="M89" s="35"/>
+      <c r="A89" s="44"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="41"/>
+      <c r="D89" s="41"/>
+      <c r="E89" s="42"/>
+      <c r="F89" s="58"/>
+      <c r="G89" s="58"/>
+      <c r="H89" s="58"/>
+      <c r="J89"/>
+      <c r="K89"/>
+      <c r="L89"/>
     </row>
     <row r="90" spans="1:13">
-      <c r="A90" s="13"/>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
-      <c r="E90" s="13"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13"/>
+      <c r="A90"/>
+      <c r="B90"/>
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+      <c r="J90"/>
     </row>
     <row r="91" spans="1:13">
-      <c r="A91" s="13"/>
-      <c r="B91" s="13" t="s">
+      <c r="A91"/>
+      <c r="B91" t="s">
         <v>69</v>
       </c>
-      <c r="C91" s="13"/>
-      <c r="D91" s="13"/>
-      <c r="E91" s="13"/>
-      <c r="F91" s="13"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91"/>
+      <c r="H91"/>
+      <c r="I91"/>
+      <c r="J91"/>
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B92" s="14"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14"/>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
-      <c r="I92" s="14"/>
-      <c r="J92" s="14"/>
-      <c r="K92" s="14"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="13"/>
+      <c r="K92" s="13"/>
       <c r="L92" s="6"/>
-      <c r="M92" s="15"/>
+      <c r="M92" s="14"/>
     </row>
     <row r="93" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A93" s="97" t="s">
+      <c r="A93" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="B93" s="97" t="s">
+      <c r="B93" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="C93" s="96" t="s">
+      <c r="C93" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="D93" s="96" t="s">
+      <c r="D93" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="E93" s="96" t="s">
+      <c r="E93" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="F93" s="107"/>
-      <c r="G93" s="107"/>
-      <c r="H93" s="107"/>
-      <c r="I93" s="109"/>
-      <c r="J93" s="96"/>
-      <c r="K93" s="16"/>
-      <c r="L93" s="17"/>
+      <c r="F93" s="97"/>
+      <c r="G93" s="97"/>
+      <c r="H93" s="97"/>
+      <c r="I93" s="99"/>
+      <c r="J93" s="86"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="16"/>
       <c r="M93" s="9"/>
     </row>
     <row r="94" spans="1:13">
-      <c r="A94" s="97"/>
-      <c r="B94" s="97"/>
-      <c r="C94" s="96"/>
-      <c r="D94" s="96"/>
-      <c r="E94" s="96"/>
-      <c r="F94" s="108"/>
-      <c r="G94" s="108"/>
-      <c r="H94" s="108"/>
-      <c r="I94" s="109"/>
-      <c r="J94" s="96"/>
-      <c r="K94" s="18"/>
-      <c r="L94" s="29"/>
-      <c r="M94" s="15"/>
+      <c r="A94" s="87"/>
+      <c r="B94" s="87"/>
+      <c r="C94" s="86"/>
+      <c r="D94" s="86"/>
+      <c r="E94" s="86"/>
+      <c r="F94" s="98"/>
+      <c r="G94" s="98"/>
+      <c r="H94" s="98"/>
+      <c r="I94" s="99"/>
+      <c r="J94" s="86"/>
+      <c r="K94" s="17"/>
+      <c r="L94" s="28"/>
+      <c r="M94" s="14"/>
     </row>
     <row r="95" spans="1:13">
-      <c r="A95" s="19">
+      <c r="A95" s="18">
         <v>1</v>
       </c>
-      <c r="B95" s="71"/>
-      <c r="C95" s="78"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="90"/>
-      <c r="G95" s="92"/>
-      <c r="H95" s="92"/>
-      <c r="I95" s="90"/>
-      <c r="J95" s="21"/>
-      <c r="K95" s="21"/>
-      <c r="L95" s="28"/>
-      <c r="M95" s="15"/>
+      <c r="B95" s="61"/>
+      <c r="C95" s="68"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="80"/>
+      <c r="G95" s="82"/>
+      <c r="H95" s="82"/>
+      <c r="I95" s="80"/>
+      <c r="J95" s="20"/>
+      <c r="K95" s="20"/>
+      <c r="L95" s="27"/>
+      <c r="M95" s="14"/>
     </row>
     <row r="96" spans="1:13">
-      <c r="A96" s="19">
+      <c r="A96" s="18">
         <f>A95+1</f>
         <v>2</v>
       </c>
-      <c r="B96" s="71"/>
-      <c r="C96" s="78"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="90"/>
-      <c r="G96" s="92"/>
-      <c r="H96" s="92"/>
-      <c r="I96" s="90"/>
-      <c r="J96" s="21"/>
-      <c r="K96" s="21"/>
-      <c r="L96" s="28"/>
-      <c r="M96" s="15"/>
+      <c r="B96" s="61"/>
+      <c r="C96" s="68"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="80"/>
+      <c r="G96" s="82"/>
+      <c r="H96" s="82"/>
+      <c r="I96" s="80"/>
+      <c r="J96" s="20"/>
+      <c r="K96" s="20"/>
+      <c r="L96" s="27"/>
+      <c r="M96" s="14"/>
     </row>
     <row r="97" spans="1:13">
-      <c r="A97" s="19">
+      <c r="A97" s="18">
         <f t="shared" ref="A97:A101" si="1">A96+1</f>
         <v>3</v>
       </c>
-      <c r="B97" s="72"/>
-      <c r="C97" s="79"/>
-      <c r="D97" s="20"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="90"/>
-      <c r="G97" s="92"/>
-      <c r="H97" s="92"/>
-      <c r="I97" s="90"/>
-      <c r="J97" s="21"/>
-      <c r="K97" s="21"/>
-      <c r="L97" s="22"/>
-      <c r="M97" s="15"/>
+      <c r="B97" s="62"/>
+      <c r="C97" s="69"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="80"/>
+      <c r="G97" s="82"/>
+      <c r="H97" s="82"/>
+      <c r="I97" s="80"/>
+      <c r="J97" s="20"/>
+      <c r="K97" s="20"/>
+      <c r="L97" s="21"/>
+      <c r="M97" s="14"/>
     </row>
     <row r="98" spans="1:13">
-      <c r="A98" s="19">
+      <c r="A98" s="18">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B98" s="73"/>
-      <c r="C98" s="80"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="20"/>
-      <c r="F98" s="90"/>
-      <c r="G98" s="92"/>
-      <c r="H98" s="92"/>
-      <c r="I98" s="90"/>
-      <c r="J98" s="21"/>
-      <c r="K98" s="21"/>
-      <c r="L98" s="22"/>
-      <c r="M98" s="15"/>
+      <c r="B98" s="63"/>
+      <c r="C98" s="70"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="80"/>
+      <c r="G98" s="82"/>
+      <c r="H98" s="82"/>
+      <c r="I98" s="80"/>
+      <c r="J98" s="20"/>
+      <c r="K98" s="20"/>
+      <c r="L98" s="21"/>
+      <c r="M98" s="14"/>
     </row>
     <row r="99" spans="1:13">
-      <c r="A99" s="19">
+      <c r="A99" s="18">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B99" s="73"/>
-      <c r="C99" s="80"/>
-      <c r="D99" s="20"/>
-      <c r="E99" s="20"/>
-      <c r="F99" s="90"/>
-      <c r="G99" s="92"/>
-      <c r="H99" s="92"/>
-      <c r="I99" s="90"/>
-      <c r="J99" s="21"/>
-      <c r="K99" s="21"/>
-      <c r="L99" s="22"/>
-      <c r="M99" s="15"/>
+      <c r="B99" s="63"/>
+      <c r="C99" s="70"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="80"/>
+      <c r="G99" s="82"/>
+      <c r="H99" s="82"/>
+      <c r="I99" s="80"/>
+      <c r="J99" s="20"/>
+      <c r="K99" s="20"/>
+      <c r="L99" s="21"/>
+      <c r="M99" s="14"/>
     </row>
     <row r="100" spans="1:13">
-      <c r="A100" s="19">
+      <c r="A100" s="18">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B100" s="73"/>
-      <c r="C100" s="80"/>
-      <c r="D100" s="74"/>
-      <c r="E100" s="74"/>
-      <c r="F100" s="91"/>
-      <c r="G100" s="93"/>
-      <c r="H100" s="93"/>
-      <c r="I100" s="91"/>
-      <c r="J100" s="76"/>
-      <c r="K100" s="76"/>
-      <c r="L100" s="77"/>
-      <c r="M100" s="15"/>
+      <c r="B100" s="63"/>
+      <c r="C100" s="70"/>
+      <c r="D100" s="64"/>
+      <c r="E100" s="64"/>
+      <c r="F100" s="81"/>
+      <c r="G100" s="83"/>
+      <c r="H100" s="83"/>
+      <c r="I100" s="81"/>
+      <c r="J100" s="66"/>
+      <c r="K100" s="66"/>
+      <c r="L100" s="67"/>
+      <c r="M100" s="14"/>
     </row>
     <row r="101" spans="1:13">
-      <c r="A101" s="19">
+      <c r="A101" s="18">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B101" s="73"/>
-      <c r="C101" s="80"/>
-      <c r="D101" s="20"/>
-      <c r="E101" s="20"/>
-      <c r="F101" s="90"/>
-      <c r="G101" s="92"/>
-      <c r="H101" s="92"/>
-      <c r="I101" s="90"/>
-      <c r="J101" s="21"/>
-      <c r="K101" s="21"/>
-      <c r="L101" s="22"/>
-      <c r="M101" s="15"/>
+      <c r="B101" s="63"/>
+      <c r="C101" s="70"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="80"/>
+      <c r="G101" s="82"/>
+      <c r="H101" s="82"/>
+      <c r="I101" s="80"/>
+      <c r="J101" s="20"/>
+      <c r="K101" s="20"/>
+      <c r="L101" s="21"/>
+      <c r="M101" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="27">
@@ -3929,79 +3793,79 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="55" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="55" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="55" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="55" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="55" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
-    <col min="11" max="251" width="8.83203125" style="55" customWidth="1"/>
-    <col min="252" max="16384" width="10.83203125" style="55"/>
+    <col min="1" max="3" width="8.83203125" style="47" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="47" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="47" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="47" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="11" max="251" width="8.83203125" style="47" customWidth="1"/>
+    <col min="252" max="16384" width="10.83203125" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="54" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="48" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="J4" s="58"/>
+      <c r="F4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="J4" s="50"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="60"/>
-      <c r="F5" s="60" t="s">
+      <c r="D5" s="52"/>
+      <c r="F5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="60" t="s">
+      <c r="H5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="52" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="61"/>
+      <c r="B6" s="53"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6"/>

</xml_diff>